<commit_message>
Stand for KSM 2016
</commit_message>
<xml_diff>
--- a/src/main/resources/kegelmeisterschaft/service/importer/2015/player/Auf die Buben.xlsx
+++ b/src/main/resources/kegelmeisterschaft/service/importer/2015/player/Auf die Buben.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId3"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>firstName</t>
   </si>
@@ -25,7 +25,7 @@
     <t>singleRelevant</t>
   </si>
   <si>
-    <t>Gurdrun</t>
+    <t>Gudrun</t>
   </si>
   <si>
     <t>Grote</t>
@@ -40,43 +40,28 @@
     <t>Todtenhöfer</t>
   </si>
   <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
     <t>Elsbeth</t>
   </si>
   <si>
     <t>Holzminden</t>
   </si>
   <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
     <t>Irene</t>
   </si>
   <si>
     <t>Paschke</t>
   </si>
   <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
     <t>Ulla</t>
   </si>
   <si>
     <t>Baumann</t>
   </si>
   <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
     <t>Waltraut</t>
   </si>
   <si>
     <t>Hoffmann</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
   </si>
 </sst>
 </file>
@@ -123,25 +108,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
-    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1" applyFill="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -157,100 +142,100 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c t="s" s="1" r="A1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="C1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c t="s" s="2" r="A2">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="2" r="C2">
-        <v>6</v>
-      </c>
-      <c t="b" s="2" r="D2">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c t="s" s="2" r="A3">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="3" r="B3">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="b" s="2" r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c t="s" s="2" r="A4">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="b" s="2" r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c t="s" s="2" r="A5">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="B5">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c t="b" s="2" r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c t="s" s="2" r="A6">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="2" r="B6">
-        <v>17</v>
-      </c>
-      <c t="s" s="2" r="C6">
-        <v>18</v>
-      </c>
-      <c t="b" s="2" r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c t="s" s="2" r="A7">
-        <v>19</v>
-      </c>
-      <c t="s" s="2" r="B7">
-        <v>20</v>
-      </c>
-      <c t="s" s="2" r="C7">
-        <v>21</v>
-      </c>
-      <c t="b" s="2" r="D7">
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>